<commit_message>
Updated GVK's Road No 47 (2077 Sq Yards )
</commit_message>
<xml_diff>
--- a/Calculate.xlsx
+++ b/Calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a063b81c7d42b926/Documents/ASR-Props/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{4AC29497-7BDA-F04A-BC42-EEECDED25249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B95C6123-6D06-49CF-8CF0-34D8A6816628}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="8_{4AC29497-7BDA-F04A-BC42-EEECDED25249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF427219-91BD-0C48-9CD6-39B0C0271A50}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -69,10 +80,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0"/>
-    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0;[Red]&quot;₹&quot;\ #,##0"/>
-    <numFmt numFmtId="167" formatCode="&quot;₹&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;₹&quot;\ #,##0;[Red]&quot;₹&quot;\ #,##0"/>
+    <numFmt numFmtId="166" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -312,18 +323,18 @@
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -335,13 +346,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -352,7 +363,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -361,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -681,20 +692,20 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.71484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
@@ -705,7 +716,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
@@ -713,7 +724,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
@@ -722,11 +733,11 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>10</v>
       </c>
@@ -734,30 +745,30 @@
         <v>8</v>
       </c>
       <c r="C6" s="17">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="10">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="12">
         <f>C6*C7</f>
-        <v>192000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>405160000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>12</v>
       </c>
@@ -775,7 +786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>3</v>
       </c>
@@ -784,7 +795,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
@@ -793,8 +804,8 @@
         <v>166666.66666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>13</v>
       </c>
@@ -806,7 +817,7 @@
         <v>400000000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="19">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -815,7 +826,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B16" s="18">
         <v>0.01</v>
       </c>
@@ -824,7 +835,7 @@
         <v>4000000</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20">
         <v>7.4999999999999997E-3</v>
       </c>

</xml_diff>